<commit_message>
CLI Version without special features
</commit_message>
<xml_diff>
--- a/emails.xlsx
+++ b/emails.xlsx
@@ -1,34 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabiansykes/Documents/GitHub/Simple_MailGenerator/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A499DBDA-C83E-164E-BD3A-22C6E09FBC9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="1480" yWindow="500" windowWidth="34660" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -47,80 +55,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -408,104 +357,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="O37" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Fabian.Sykes@example.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>FabianSykes@example.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Fabian_Sykes@example.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Test.Test@example.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>TestTest@example.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Test_Test@example.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Username.User@example.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>UsernameUser@example.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Username_User@example.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>sadad.asdasd@example.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>sadadasdasd@example.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>sadad_asdasd@example.com</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added "open in Excel" button
</commit_message>
<xml_diff>
--- a/emails.xlsx
+++ b/emails.xlsx
@@ -1,42 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabiansykes/Documents/GitHub/Simple_MailGenerator/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C57D5C2-DA1A-3645-804A-F278F0313699}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="500" windowWidth="35840" windowHeight="22400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -55,21 +47,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -357,15 +408,300 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>test.test@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>testtest@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>test_test@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>t.test@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>test.t@gmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>test.test@yahoo.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>testtest@yahoo.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>test_test@yahoo.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>t.test@yahoo.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>test.t@yahoo.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>test.test@hotmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>testtest@hotmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>test_test@hotmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>t.test@hotmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>test.t@hotmail.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>test.test@aon.at</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>testtest@aon.at</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>test_test@aon.at</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>t.test@aon.at</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>test.t@aon.at</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>test.test@gmx.at</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>testtest@gmx.at</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>test_test@gmx.at</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>t.test@gmx.at</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>test.t@gmx.at</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>test.test@outlook.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>testtest@outlook.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>test_test@outlook.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>t.test@outlook.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>test.t@outlook.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>test.test@live.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>testtest@live.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>test_test@live.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>t.test@live.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>test.t@live.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>test.test@icloud.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>testtest@icloud.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>test_test@icloud.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>t.test@icloud.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>test.t@icloud.com</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>